<commit_message>
Updating of "main" branch with the definitive version of the simulator
</commit_message>
<xml_diff>
--- a/mapa_balizas.xlsx
+++ b/mapa_balizas.xlsx
@@ -5,22 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Master\Guiado\code_balizas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Desktop\Alberto\Master_Automatica_Robotica_UPM\Guiado_y_Navegacion\Autonomous_Surveillance_Robot_Iss5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C3ADA-F5B4-44AD-B078-6F68F66A76B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532C2A23-B508-4D4B-9502-98FF468CF253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,15 +354,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0.05</v>
       </c>
@@ -374,7 +370,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2.5</v>
       </c>
@@ -382,7 +378,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.05</v>
       </c>
@@ -390,7 +386,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14.95</v>
       </c>
@@ -398,7 +394,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>15</v>
       </c>
@@ -406,7 +402,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>15</v>
       </c>
@@ -414,7 +410,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.05</v>
       </c>
@@ -422,7 +418,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7.5</v>
       </c>
@@ -430,7 +426,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20</v>
       </c>
@@ -438,7 +434,7 @@
         <v>12.45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15.05</v>
       </c>
@@ -446,7 +442,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -454,7 +450,7 @@
         <v>12.55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15.05</v>
       </c>
@@ -462,7 +458,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11.55</v>
       </c>
@@ -470,7 +466,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.05</v>
       </c>
@@ -478,7 +474,7 @@
         <v>39.950000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9.9499999999999993</v>
       </c>
@@ -486,7 +482,7 @@
         <v>25.05</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10.050000000000001</v>
       </c>
@@ -494,7 +490,7 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>39.950000000000003</v>
       </c>
@@ -502,7 +498,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>37.5</v>
       </c>
@@ -510,7 +506,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>39.950000000000003</v>
       </c>
@@ -518,7 +514,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>24.95</v>
       </c>
@@ -526,7 +522,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -534,7 +530,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>25</v>
       </c>
@@ -542,7 +538,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>39.950000000000003</v>
       </c>
@@ -550,7 +546,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>32.5</v>
       </c>
@@ -558,7 +554,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25.05</v>
       </c>
@@ -566,7 +562,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>35.049999999999997</v>
       </c>
@@ -574,7 +570,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>30</v>
       </c>
@@ -582,7 +578,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>39.950000000000003</v>
       </c>
@@ -590,7 +586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -598,7 +594,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -606,7 +602,7 @@
         <v>32.450000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -614,7 +610,7 @@
         <v>37.549999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.05</v>
       </c>
@@ -622,12 +618,28 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0.05</v>
       </c>
       <c r="B33">
         <v>25.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>29.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>19.95</v>
+      </c>
+      <c r="B35">
+        <v>39.950000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>